<commit_message>
sofia | bulkheads curve | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_Holds_curve.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_Holds_curve.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548EF53C-4A65-4352-B97D-06B2C3A99E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF1D13D-C835-4727-9D9A-F541B5661684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" firstSheet="3" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Трюм 101 (H101)" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="9">
   <si>
     <t>Depth of cargo [m]</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>0 00</t>
-  </si>
-  <si>
-    <t>6 35</t>
   </si>
   <si>
     <t xml:space="preserve">25,58 </t>
@@ -168,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,6 +187,9 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1593,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -1633,7 +1633,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1813,7 +1813,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1853,7 +1853,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1873,7 +1873,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.83</v>
       </c>
     </row>
@@ -1933,7 +1933,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.95</v>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -1973,7 +1973,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       <c r="E23" s="1">
         <v>6.35</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -2033,7 +2033,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -2048,7 +2048,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D2" sqref="D2:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2098,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2118,7 +2118,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -2138,7 +2138,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -2158,7 +2158,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -2218,7 +2218,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -2238,7 +2238,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2258,7 +2258,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2278,7 +2278,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2298,7 +2298,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2318,7 +2318,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2358,7 +2358,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2378,7 +2378,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2398,7 +2398,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.83</v>
       </c>
     </row>
@@ -2438,7 +2438,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.95</v>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -2518,7 +2518,7 @@
       <c r="E23" s="1">
         <v>6.35</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -2538,7 +2538,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -2553,7 +2553,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,17 +2593,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="7">
-        <f t="shared" ref="C2:D2" si="0">C3</f>
-        <v>96.88</v>
+        <v>92.92</v>
       </c>
       <c r="D2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D2" si="0">D3</f>
         <v>0</v>
       </c>
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -2614,8 +2613,8 @@
       <c r="B3" s="1">
         <v>4.37</v>
       </c>
-      <c r="C3" s="1">
-        <v>96.88</v>
+      <c r="C3" s="8">
+        <v>92.92</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -2623,7 +2622,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -2634,8 +2633,8 @@
       <c r="B4" s="1">
         <v>8.73</v>
       </c>
-      <c r="C4" s="1">
-        <v>96.88</v>
+      <c r="C4" s="7">
+        <v>92.92</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -2643,7 +2642,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -2654,8 +2653,8 @@
       <c r="B5" s="1">
         <v>13.1</v>
       </c>
-      <c r="C5" s="1">
-        <v>96.88</v>
+      <c r="C5" s="8">
+        <v>92.92</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -2663,7 +2662,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -2674,8 +2673,8 @@
       <c r="B6" s="1">
         <v>17.46</v>
       </c>
-      <c r="C6" s="1">
-        <v>96.88</v>
+      <c r="C6" s="7">
+        <v>92.92</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -2683,7 +2682,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -2694,8 +2693,8 @@
       <c r="B7" s="1">
         <v>21.83</v>
       </c>
-      <c r="C7" s="1">
-        <v>96.88</v>
+      <c r="C7" s="8">
+        <v>92.92</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -2703,7 +2702,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -2714,8 +2713,8 @@
       <c r="B8" s="1">
         <v>26.2</v>
       </c>
-      <c r="C8" s="1">
-        <v>96.88</v>
+      <c r="C8" s="7">
+        <v>92.92</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -2723,7 +2722,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -2734,8 +2733,8 @@
       <c r="B9" s="1">
         <v>30.56</v>
       </c>
-      <c r="C9" s="1">
-        <v>96.88</v>
+      <c r="C9" s="8">
+        <v>92.92</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -2743,7 +2742,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2754,8 +2753,8 @@
       <c r="B10" s="1">
         <v>34.93</v>
       </c>
-      <c r="C10" s="1">
-        <v>96.88</v>
+      <c r="C10" s="7">
+        <v>92.92</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -2763,7 +2762,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2774,8 +2773,8 @@
       <c r="B11" s="1">
         <v>39.299999999999997</v>
       </c>
-      <c r="C11" s="1">
-        <v>96.88</v>
+      <c r="C11" s="8">
+        <v>92.92</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -2783,7 +2782,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2794,8 +2793,8 @@
       <c r="B12" s="1">
         <v>43.66</v>
       </c>
-      <c r="C12" s="1">
-        <v>96.88</v>
+      <c r="C12" s="7">
+        <v>92.92</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -2803,7 +2802,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2814,8 +2813,8 @@
       <c r="B13" s="1">
         <v>48.03</v>
       </c>
-      <c r="C13" s="1">
-        <v>96.88</v>
+      <c r="C13" s="8">
+        <v>92.92</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -2823,7 +2822,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2834,8 +2833,8 @@
       <c r="B14" s="1">
         <v>52.39</v>
       </c>
-      <c r="C14" s="1">
-        <v>96.88</v>
+      <c r="C14" s="7">
+        <v>92.92</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -2843,7 +2842,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2854,8 +2853,8 @@
       <c r="B15" s="1">
         <v>56.76</v>
       </c>
-      <c r="C15" s="1">
-        <v>96.88</v>
+      <c r="C15" s="8">
+        <v>92.92</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -2863,7 +2862,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2874,8 +2873,8 @@
       <c r="B16" s="1">
         <v>61.13</v>
       </c>
-      <c r="C16" s="1">
-        <v>96.88</v>
+      <c r="C16" s="7">
+        <v>92.92</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -2883,7 +2882,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2894,8 +2893,8 @@
       <c r="B17" s="1">
         <v>65.489999999999995</v>
       </c>
-      <c r="C17" s="1">
-        <v>96.88</v>
+      <c r="C17" s="8">
+        <v>92.92</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -2903,7 +2902,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -2914,8 +2913,8 @@
       <c r="B18" s="1">
         <v>69.86</v>
       </c>
-      <c r="C18" s="1">
-        <v>96.88</v>
+      <c r="C18" s="7">
+        <v>92.92</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -2923,7 +2922,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.819999999999993</v>
       </c>
     </row>
@@ -2934,8 +2933,8 @@
       <c r="B19" s="1">
         <v>74.22</v>
       </c>
-      <c r="C19" s="1">
-        <v>96.88</v>
+      <c r="C19" s="8">
+        <v>92.92</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -2943,7 +2942,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.94</v>
       </c>
     </row>
@@ -2954,8 +2953,8 @@
       <c r="B20" s="1">
         <v>78.59</v>
       </c>
-      <c r="C20" s="1">
-        <v>96.88</v>
+      <c r="C20" s="7">
+        <v>92.92</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -2963,7 +2962,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -2974,8 +2973,8 @@
       <c r="B21" s="1">
         <v>82.96</v>
       </c>
-      <c r="C21" s="1">
-        <v>96.88</v>
+      <c r="C21" s="8">
+        <v>92.92</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -2983,7 +2982,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -2994,8 +2993,8 @@
       <c r="B22" s="1">
         <v>87.32</v>
       </c>
-      <c r="C22" s="1">
-        <v>96.88</v>
+      <c r="C22" s="7">
+        <v>92.92</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -3003,7 +3002,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -3014,8 +3013,8 @@
       <c r="B23" s="1">
         <v>91.69</v>
       </c>
-      <c r="C23" s="1">
-        <v>96.88</v>
+      <c r="C23" s="8">
+        <v>92.92</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -3023,7 +3022,7 @@
       <c r="E23" s="1">
         <v>6.35</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -3034,8 +3033,8 @@
       <c r="B24" s="1">
         <v>94.35</v>
       </c>
-      <c r="C24" s="1">
-        <v>96.88</v>
+      <c r="C24" s="8">
+        <v>92.92</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -3043,7 +3042,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -3058,7 +3057,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F2" sqref="F2:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,7 +3107,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3128,7 +3127,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -3148,7 +3147,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -3168,7 +3167,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -3188,7 +3187,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -3208,7 +3207,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -3228,7 +3227,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -3248,7 +3247,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3268,7 +3267,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3288,7 +3287,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3308,7 +3307,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3328,7 +3327,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3348,7 +3347,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3368,7 +3367,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3388,7 +3387,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3408,7 +3407,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3428,7 +3427,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.819999999999993</v>
       </c>
     </row>
@@ -3448,7 +3447,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.94</v>
       </c>
     </row>
@@ -3468,7 +3467,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -3488,7 +3487,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -3508,7 +3507,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.250999999999998</v>
       </c>
     </row>
@@ -3528,7 +3527,7 @@
       <c r="E23" s="1">
         <v>6.35</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -3548,7 +3547,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -3563,7 +3562,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3612,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3633,7 +3632,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -3653,7 +3652,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -3673,7 +3672,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -3693,7 +3692,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -3713,7 +3712,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -3733,7 +3732,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -3753,7 +3752,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3773,7 +3772,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3793,7 +3792,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3813,7 +3812,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3833,7 +3832,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3853,7 +3852,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3873,7 +3872,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3893,7 +3892,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3913,7 +3912,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -3933,7 +3932,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.819999999999993</v>
       </c>
     </row>
@@ -3953,7 +3952,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.94</v>
       </c>
     </row>
@@ -3973,7 +3972,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -3993,7 +3992,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -4013,7 +4012,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -4033,7 +4032,7 @@
       <c r="E23" s="1">
         <v>6.35</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -4053,7 +4052,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -4068,7 +4067,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4118,7 +4117,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -4138,7 +4137,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -4158,7 +4157,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -4178,7 +4177,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -4198,7 +4197,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -4218,7 +4217,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -4238,7 +4237,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -4258,7 +4257,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4278,7 +4277,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4298,7 +4297,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4318,7 +4317,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4338,7 +4337,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4358,7 +4357,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4378,7 +4377,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4398,7 +4397,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4418,7 +4417,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4438,7 +4437,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.819999999999993</v>
       </c>
     </row>
@@ -4458,7 +4457,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.94</v>
       </c>
     </row>
@@ -4478,7 +4477,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -4498,7 +4497,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -4518,7 +4517,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -4535,10 +4534,10 @@
       <c r="D23" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="E23" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -4558,7 +4557,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -4573,7 +4572,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4623,7 +4622,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -4643,7 +4642,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -4663,7 +4662,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -4683,7 +4682,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -4703,7 +4702,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -4723,7 +4722,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -4743,7 +4742,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -4763,7 +4762,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4783,7 +4782,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4803,7 +4802,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4823,7 +4822,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4843,7 +4842,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4863,7 +4862,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4883,7 +4882,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4903,7 +4902,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4912,7 +4911,7 @@
         <v>7.5</v>
       </c>
       <c r="B17" s="1">
-        <v>61.13</v>
+        <v>65.489999999999995</v>
       </c>
       <c r="C17" s="1">
         <v>31.5</v>
@@ -4921,9 +4920,9 @@
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F17" s="2">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -4932,7 +4931,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>65.489999999999995</v>
+        <v>69.86</v>
       </c>
       <c r="C18" s="1">
         <v>31.5</v>
@@ -4941,10 +4940,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="F18" s="2">
-        <v>66.22</v>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F18" s="1">
+        <v>66.819999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4952,18 +4951,18 @@
         <v>8.5</v>
       </c>
       <c r="B19" s="1">
-        <v>69.86</v>
+        <v>74.23</v>
       </c>
       <c r="C19" s="1">
         <v>31.5</v>
       </c>
       <c r="D19" s="1">
-        <v>5.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="F19" s="2">
+        <v>5.35</v>
+      </c>
+      <c r="F19" s="1">
         <v>62.94</v>
       </c>
     </row>
@@ -4975,15 +4974,15 @@
         <v>78.59</v>
       </c>
       <c r="C20" s="1">
-        <v>41.86</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>31.5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -4995,7 +4994,7 @@
         <v>82.96</v>
       </c>
       <c r="C21" s="1">
-        <v>41.86</v>
+        <v>31.5</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -5003,7 +5002,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -5015,7 +5014,7 @@
         <v>87.32</v>
       </c>
       <c r="C22" s="1">
-        <v>41.86</v>
+        <v>31.5</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -5023,7 +5022,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -5035,15 +5034,15 @@
         <v>91.69</v>
       </c>
       <c r="C23" s="1">
-        <v>41.86</v>
+        <v>31.5</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="E23" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -5055,7 +5054,7 @@
         <v>94.35</v>
       </c>
       <c r="C24" s="1">
-        <v>41.86</v>
+        <v>31.5</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -5063,7 +5062,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -5077,8 +5076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5128,7 +5127,7 @@
       <c r="E2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -5148,7 +5147,7 @@
       <c r="E3" s="1">
         <v>1.35</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>23.6</v>
       </c>
     </row>
@@ -5168,7 +5167,7 @@
       <c r="E4" s="1">
         <v>1.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>40.020000000000003</v>
       </c>
     </row>
@@ -5188,7 +5187,7 @@
       <c r="E5" s="1">
         <v>1.85</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>51.76</v>
       </c>
     </row>
@@ -5208,7 +5207,7 @@
       <c r="E6" s="1">
         <v>2.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>59.72</v>
       </c>
     </row>
@@ -5228,7 +5227,7 @@
       <c r="E7" s="1">
         <v>2.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>64.41</v>
       </c>
     </row>
@@ -5248,7 +5247,7 @@
       <c r="E8" s="1">
         <v>2.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>66.19</v>
       </c>
     </row>
@@ -5268,7 +5267,7 @@
       <c r="E9" s="1">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5288,7 +5287,7 @@
       <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5308,7 +5307,7 @@
       <c r="E11" s="1">
         <v>3.35</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5328,7 +5327,7 @@
       <c r="E12" s="1">
         <v>3.6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5348,7 +5347,7 @@
       <c r="E13" s="1">
         <v>3.85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5368,7 +5367,7 @@
       <c r="E14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5388,7 +5387,7 @@
       <c r="E15" s="1">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5408,7 +5407,7 @@
       <c r="E16" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5428,7 +5427,7 @@
       <c r="E17" s="1">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>66.22</v>
       </c>
     </row>
@@ -5448,7 +5447,7 @@
       <c r="E18" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>65.819999999999993</v>
       </c>
     </row>
@@ -5468,7 +5467,7 @@
       <c r="E19" s="1">
         <v>5.35</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>62.94</v>
       </c>
     </row>
@@ -5488,7 +5487,7 @@
       <c r="E20" s="1">
         <v>5.6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>57.03</v>
       </c>
     </row>
@@ -5508,7 +5507,7 @@
       <c r="E21" s="1">
         <v>5.85</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>47.67</v>
       </c>
     </row>
@@ -5528,7 +5527,7 @@
       <c r="E22" s="1">
         <v>6.1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>34.25</v>
       </c>
     </row>
@@ -5548,7 +5547,7 @@
       <c r="E23" s="1">
         <v>6.35</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15.56</v>
       </c>
     </row>
@@ -5560,7 +5559,7 @@
         <v>94.35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -5568,7 +5567,7 @@
       <c r="E24" s="1">
         <v>6.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>6.32</v>
       </c>
     </row>
@@ -6087,8 +6086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sofia | hold | bug fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_Holds_curve.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Loads/SSS_Sofia_Holds_curve.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF1D13D-C835-4727-9D9A-F541B5661684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23999717-5DFF-4586-B791-143C2562F2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" firstSheet="3" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="801" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Трюм 101 (H101)" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="8">
   <si>
     <t>Depth of cargo [m]</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>22 00</t>
-  </si>
-  <si>
-    <t>0 00</t>
   </si>
   <si>
     <t xml:space="preserve">25,58 </t>
@@ -4066,8 +4063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,8 +4468,8 @@
       <c r="C20" s="1">
         <v>41.86</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>7</v>
+      <c r="D20" s="1">
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <v>5.6</v>
@@ -5076,7 +5073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -5559,7 +5556,7 @@
         <v>94.35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>

</xml_diff>